<commit_message>
Mise en fonctionnement de la page interfaceCaracteristique.php
</commit_message>
<xml_diff>
--- a/fichierInter.xlsx
+++ b/fichierInter.xlsx
@@ -36,7 +36,7 @@
     <t>Date début semaine</t>
   </si>
   <si>
-    <t>Loire</t>
+    <t>Plaine</t>
   </si>
   <si>
     <t>07/01/2021</t>
@@ -775,15 +775,9 @@
       <c r="C9" t="s">
         <v>14</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>4</v>
-      </c>
-      <c r="F9">
-        <v>10.58</v>
-      </c>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
@@ -810,13 +804,13 @@
         <v>16</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="F11">
-        <v>19.08</v>
+        <v>14.15</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -830,13 +824,13 @@
         <v>17</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="F12">
-        <v>20.76</v>
+        <v>20.18</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -853,10 +847,10 @@
         <v>4</v>
       </c>
       <c r="E13">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="F13">
-        <v>18.0</v>
+        <v>24.31</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -870,13 +864,13 @@
         <v>19</v>
       </c>
       <c r="D14">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E14">
-        <v>109</v>
+        <v>166</v>
       </c>
       <c r="F14">
-        <v>31.57</v>
+        <v>32.94</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -890,13 +884,13 @@
         <v>20</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E15">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="F15">
-        <v>43.14</v>
+        <v>44.95</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -910,13 +904,13 @@
         <v>21</v>
       </c>
       <c r="D16">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E16">
-        <v>55</v>
+        <v>112</v>
       </c>
       <c r="F16">
-        <v>26.98</v>
+        <v>42.3</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -930,13 +924,13 @@
         <v>22</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E17">
-        <v>46</v>
+        <v>127</v>
       </c>
       <c r="F17">
-        <v>26.74</v>
+        <v>34.39</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -950,13 +944,13 @@
         <v>23</v>
       </c>
       <c r="D18">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E18">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="F18">
-        <v>34.47</v>
+        <v>49.96</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -970,13 +964,13 @@
         <v>24</v>
       </c>
       <c r="D19">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E19">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="F19">
-        <v>51.3</v>
+        <v>69.17</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -990,13 +984,13 @@
         <v>25</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E20">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="F20">
-        <v>29.84</v>
+        <v>70.15</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1010,13 +1004,13 @@
         <v>26</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E21">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="F21">
-        <v>71.17</v>
+        <v>81.56</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1030,13 +1024,13 @@
         <v>27</v>
       </c>
       <c r="D22">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E22">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F22">
-        <v>40.34</v>
+        <v>51.85</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1050,13 +1044,13 @@
         <v>28</v>
       </c>
       <c r="D23">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E23">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="F23">
-        <v>62.83</v>
+        <v>53.65</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1070,13 +1064,13 @@
         <v>29</v>
       </c>
       <c r="D24">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E24">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F24">
-        <v>44.42</v>
+        <v>49.95</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1090,13 +1084,13 @@
         <v>30</v>
       </c>
       <c r="D25">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E25">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="F25">
-        <v>36.02</v>
+        <v>89.1</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1113,10 +1107,10 @@
         <v>5</v>
       </c>
       <c r="E26">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F26">
-        <v>41.0</v>
+        <v>40.42</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1130,13 +1124,13 @@
         <v>32</v>
       </c>
       <c r="D27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E27">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F27">
-        <v>31.33</v>
+        <v>51.68</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1150,13 +1144,13 @@
         <v>33</v>
       </c>
       <c r="D28">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E28">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="F28">
-        <v>35.72</v>
+        <v>48.14</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1170,13 +1164,13 @@
         <v>34</v>
       </c>
       <c r="D29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="F29">
-        <v>34.52</v>
+        <v>71.43</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1189,9 +1183,15 @@
       <c r="C30" t="s">
         <v>35</v>
       </c>
-      <c r="D30"/>
-      <c r="E30"/>
-      <c r="F30"/>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>10</v>
+      </c>
+      <c r="F30">
+        <v>46.87</v>
+      </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
@@ -1203,9 +1203,15 @@
       <c r="C31" t="s">
         <v>36</v>
       </c>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>5</v>
+      </c>
+      <c r="F31">
+        <v>21.43</v>
+      </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
@@ -1231,9 +1237,15 @@
       <c r="C33" t="s">
         <v>38</v>
       </c>
-      <c r="D33"/>
-      <c r="E33"/>
-      <c r="F33"/>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+      <c r="F33">
+        <v>44.05</v>
+      </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
@@ -1245,9 +1257,15 @@
       <c r="C34" t="s">
         <v>39</v>
       </c>
-      <c r="D34"/>
-      <c r="E34"/>
-      <c r="F34"/>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>6</v>
+      </c>
+      <c r="F34">
+        <v>54.63</v>
+      </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
@@ -1259,9 +1277,15 @@
       <c r="C35" t="s">
         <v>40</v>
       </c>
-      <c r="D35"/>
-      <c r="E35"/>
-      <c r="F35"/>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>7</v>
+      </c>
+      <c r="F35">
+        <v>33.48</v>
+      </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
@@ -1277,10 +1301,10 @@
         <v>2</v>
       </c>
       <c r="E36">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F36">
-        <v>15.73</v>
+        <v>15.14</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1294,13 +1318,13 @@
         <v>42</v>
       </c>
       <c r="D37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E37">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F37">
-        <v>26.98</v>
+        <v>73.61</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1313,15 +1337,9 @@
       <c r="C38" t="s">
         <v>43</v>
       </c>
-      <c r="D38">
-        <v>2</v>
-      </c>
-      <c r="E38">
-        <v>6</v>
-      </c>
-      <c r="F38">
-        <v>17.86</v>
-      </c>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
@@ -1334,13 +1352,13 @@
         <v>44</v>
       </c>
       <c r="D39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E39">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F39">
-        <v>22.32</v>
+        <v>30.59</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1353,15 +1371,9 @@
       <c r="C40" t="s">
         <v>45</v>
       </c>
-      <c r="D40">
-        <v>2</v>
-      </c>
-      <c r="E40">
-        <v>6</v>
-      </c>
-      <c r="F40">
-        <v>17.86</v>
-      </c>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
@@ -1377,10 +1389,10 @@
         <v>1</v>
       </c>
       <c r="E41">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F41">
-        <v>35.71</v>
+        <v>22.92</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1394,13 +1406,13 @@
         <v>47</v>
       </c>
       <c r="D42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E42">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F42">
-        <v>11.11</v>
+        <v>23.47</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1417,10 +1429,10 @@
         <v>1</v>
       </c>
       <c r="E43">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F43">
-        <v>14.29</v>
+        <v>12.12</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1700,15 +1712,9 @@
       <c r="C7" t="s">
         <v>66</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7">
-        <v>10.58</v>
-      </c>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
@@ -1721,13 +1727,13 @@
         <v>16</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="F8">
-        <v>19.08</v>
+        <v>14.15</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1741,13 +1747,13 @@
         <v>67</v>
       </c>
       <c r="D9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E9">
-        <v>111</v>
+        <v>76</v>
       </c>
       <c r="F9">
-        <v>19.73</v>
+        <v>18.53</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1761,13 +1767,13 @@
         <v>68</v>
       </c>
       <c r="D10">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E10">
-        <v>85</v>
+        <v>169</v>
       </c>
       <c r="F10">
-        <v>29.59</v>
+        <v>33.02</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1781,13 +1787,13 @@
         <v>69</v>
       </c>
       <c r="D11">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E11">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="F11">
-        <v>35.55</v>
+        <v>40.35</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1801,13 +1807,13 @@
         <v>70</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E12">
-        <v>45</v>
+        <v>145</v>
       </c>
       <c r="F12">
-        <v>32.65</v>
+        <v>38.55</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1821,13 +1827,13 @@
         <v>71</v>
       </c>
       <c r="D13">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E13">
-        <v>98</v>
+        <v>179</v>
       </c>
       <c r="F13">
-        <v>34.78</v>
+        <v>50.58</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1841,13 +1847,13 @@
         <v>72</v>
       </c>
       <c r="D14">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E14">
-        <v>79</v>
+        <v>130</v>
       </c>
       <c r="F14">
-        <v>46.45</v>
+        <v>69.06</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1861,13 +1867,13 @@
         <v>26</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E15">
-        <v>44</v>
+        <v>123</v>
       </c>
       <c r="F15">
-        <v>57.87</v>
+        <v>78.95</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1881,13 +1887,13 @@
         <v>73</v>
       </c>
       <c r="D16">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E16">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F16">
-        <v>44.63</v>
+        <v>53.03</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1901,13 +1907,13 @@
         <v>74</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E17">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="F17">
-        <v>52.34</v>
+        <v>55.49</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1921,13 +1927,13 @@
         <v>75</v>
       </c>
       <c r="D18">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E18">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="F18">
-        <v>40.64</v>
+        <v>76.41</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1941,13 +1947,13 @@
         <v>76</v>
       </c>
       <c r="D19">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E19">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F19">
-        <v>33.95</v>
+        <v>43.41</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1961,13 +1967,13 @@
         <v>77</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E20">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="F20">
-        <v>35.42</v>
+        <v>50.59</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1980,9 +1986,15 @@
       <c r="C21" t="s">
         <v>78</v>
       </c>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21"/>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>7</v>
+      </c>
+      <c r="F21">
+        <v>64.58</v>
+      </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
@@ -1994,9 +2006,15 @@
       <c r="C22" t="s">
         <v>36</v>
       </c>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>8</v>
+      </c>
+      <c r="F22">
+        <v>25.3</v>
+      </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
@@ -2022,9 +2040,15 @@
       <c r="C24" t="s">
         <v>80</v>
       </c>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24"/>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>9</v>
+      </c>
+      <c r="F24">
+        <v>49.34</v>
+      </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
@@ -2040,10 +2064,10 @@
         <v>1</v>
       </c>
       <c r="E25">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F25">
-        <v>12.5</v>
+        <v>33.48</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2057,13 +2081,13 @@
         <v>82</v>
       </c>
       <c r="D26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E26">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F26">
-        <v>22.97</v>
+        <v>44.38</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2077,13 +2101,13 @@
         <v>83</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E27">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F27">
-        <v>20.09</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2097,13 +2121,13 @@
         <v>84</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28">
         <v>6</v>
       </c>
       <c r="F28">
-        <v>17.86</v>
+        <v>41.67</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2120,10 +2144,10 @@
         <v>1</v>
       </c>
       <c r="E29">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F29">
-        <v>35.71</v>
+        <v>22.92</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2137,13 +2161,13 @@
         <v>85</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F30">
-        <v>12.7</v>
+        <v>23.47</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2156,9 +2180,15 @@
       <c r="C31" t="s">
         <v>86</v>
       </c>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>6</v>
+      </c>
+      <c r="F31">
+        <v>12.12</v>
+      </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">

</xml_diff>

<commit_message>
Modification de l'interface et test de la fonction sur interface groupe exploitations
</commit_message>
<xml_diff>
--- a/fichierInter.xlsx
+++ b/fichierInter.xlsx
@@ -9,6 +9,8 @@
   <sheets>
     <sheet name="2020 Semaine" sheetId="1" r:id="rId4"/>
     <sheet name="2020 Décade" sheetId="2" r:id="rId5"/>
+    <sheet name="2021 Semaine" sheetId="3" r:id="rId6"/>
+    <sheet name="2021 Décade" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -16,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="175">
   <si>
     <t>Groupe</t>
   </si>
@@ -36,7 +38,7 @@
     <t>Date début semaine</t>
   </si>
   <si>
-    <t>Plaine</t>
+    <t>Adice</t>
   </si>
   <si>
     <t>07/01/2020</t>
@@ -292,6 +294,255 @@
   </si>
   <si>
     <t>25/12/2020</t>
+  </si>
+  <si>
+    <t>07/01/2021</t>
+  </si>
+  <si>
+    <t>14/01/2021</t>
+  </si>
+  <si>
+    <t>21/01/2021</t>
+  </si>
+  <si>
+    <t>28/01/2021</t>
+  </si>
+  <si>
+    <t>04/02/2021</t>
+  </si>
+  <si>
+    <t>11/02/2021</t>
+  </si>
+  <si>
+    <t>18/02/2021</t>
+  </si>
+  <si>
+    <t>25/02/2021</t>
+  </si>
+  <si>
+    <t>04/03/2021</t>
+  </si>
+  <si>
+    <t>11/03/2021</t>
+  </si>
+  <si>
+    <t>18/03/2021</t>
+  </si>
+  <si>
+    <t>25/03/2021</t>
+  </si>
+  <si>
+    <t>01/04/2021</t>
+  </si>
+  <si>
+    <t>08/04/2021</t>
+  </si>
+  <si>
+    <t>15/04/2021</t>
+  </si>
+  <si>
+    <t>22/04/2021</t>
+  </si>
+  <si>
+    <t>29/04/2021</t>
+  </si>
+  <si>
+    <t>06/05/2021</t>
+  </si>
+  <si>
+    <t>13/05/2021</t>
+  </si>
+  <si>
+    <t>20/05/2021</t>
+  </si>
+  <si>
+    <t>27/05/2021</t>
+  </si>
+  <si>
+    <t>03/06/2021</t>
+  </si>
+  <si>
+    <t>10/06/2021</t>
+  </si>
+  <si>
+    <t>17/06/2021</t>
+  </si>
+  <si>
+    <t>24/06/2021</t>
+  </si>
+  <si>
+    <t>01/07/2021</t>
+  </si>
+  <si>
+    <t>08/07/2021</t>
+  </si>
+  <si>
+    <t>15/07/2021</t>
+  </si>
+  <si>
+    <t>22/07/2021</t>
+  </si>
+  <si>
+    <t>29/07/2021</t>
+  </si>
+  <si>
+    <t>05/08/2021</t>
+  </si>
+  <si>
+    <t>12/08/2021</t>
+  </si>
+  <si>
+    <t>19/08/2021</t>
+  </si>
+  <si>
+    <t>26/08/2021</t>
+  </si>
+  <si>
+    <t>02/09/2021</t>
+  </si>
+  <si>
+    <t>09/09/2021</t>
+  </si>
+  <si>
+    <t>16/09/2021</t>
+  </si>
+  <si>
+    <t>23/09/2021</t>
+  </si>
+  <si>
+    <t>30/09/2021</t>
+  </si>
+  <si>
+    <t>07/10/2021</t>
+  </si>
+  <si>
+    <t>14/10/2021</t>
+  </si>
+  <si>
+    <t>21/10/2021</t>
+  </si>
+  <si>
+    <t>28/10/2021</t>
+  </si>
+  <si>
+    <t>04/11/2021</t>
+  </si>
+  <si>
+    <t>11/11/2021</t>
+  </si>
+  <si>
+    <t>18/11/2021</t>
+  </si>
+  <si>
+    <t>25/11/2021</t>
+  </si>
+  <si>
+    <t>02/12/2021</t>
+  </si>
+  <si>
+    <t>09/12/2021</t>
+  </si>
+  <si>
+    <t>16/12/2021</t>
+  </si>
+  <si>
+    <t>23/12/2021</t>
+  </si>
+  <si>
+    <t>30/12/2021</t>
+  </si>
+  <si>
+    <t>10/01/2021</t>
+  </si>
+  <si>
+    <t>20/01/2021</t>
+  </si>
+  <si>
+    <t>30/01/2021</t>
+  </si>
+  <si>
+    <t>09/02/2021</t>
+  </si>
+  <si>
+    <t>19/02/2021</t>
+  </si>
+  <si>
+    <t>01/03/2021</t>
+  </si>
+  <si>
+    <t>21/03/2021</t>
+  </si>
+  <si>
+    <t>31/03/2021</t>
+  </si>
+  <si>
+    <t>10/04/2021</t>
+  </si>
+  <si>
+    <t>20/04/2021</t>
+  </si>
+  <si>
+    <t>30/04/2021</t>
+  </si>
+  <si>
+    <t>10/05/2021</t>
+  </si>
+  <si>
+    <t>30/05/2021</t>
+  </si>
+  <si>
+    <t>09/06/2021</t>
+  </si>
+  <si>
+    <t>19/06/2021</t>
+  </si>
+  <si>
+    <t>29/06/2021</t>
+  </si>
+  <si>
+    <t>09/07/2021</t>
+  </si>
+  <si>
+    <t>19/07/2021</t>
+  </si>
+  <si>
+    <t>08/08/2021</t>
+  </si>
+  <si>
+    <t>18/08/2021</t>
+  </si>
+  <si>
+    <t>28/08/2021</t>
+  </si>
+  <si>
+    <t>07/09/2021</t>
+  </si>
+  <si>
+    <t>17/09/2021</t>
+  </si>
+  <si>
+    <t>27/09/2021</t>
+  </si>
+  <si>
+    <t>17/10/2021</t>
+  </si>
+  <si>
+    <t>27/10/2021</t>
+  </si>
+  <si>
+    <t>06/11/2021</t>
+  </si>
+  <si>
+    <t>16/11/2021</t>
+  </si>
+  <si>
+    <t>26/11/2021</t>
+  </si>
+  <si>
+    <t>06/12/2021</t>
+  </si>
+  <si>
+    <t>26/12/2021</t>
   </si>
 </sst>
 </file>
@@ -775,15 +1026,9 @@
       <c r="C9" t="s">
         <v>14</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>8</v>
-      </c>
-      <c r="F9">
-        <v>21.25</v>
-      </c>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
@@ -795,15 +1040,9 @@
       <c r="C10" t="s">
         <v>15</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>17</v>
-      </c>
-      <c r="F10">
-        <v>15.13</v>
-      </c>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
@@ -816,13 +1055,13 @@
         <v>16</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F11">
-        <v>35.42</v>
+        <v>3.13</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -839,10 +1078,10 @@
         <v>2</v>
       </c>
       <c r="E12">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="F12">
-        <v>25.89</v>
+        <v>17.68</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -856,13 +1095,13 @@
         <v>18</v>
       </c>
       <c r="D13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E13">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="F13">
-        <v>51.02</v>
+        <v>25.98</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -876,13 +1115,13 @@
         <v>19</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E14">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="F14">
-        <v>38.4</v>
+        <v>28.51</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -896,13 +1135,13 @@
         <v>20</v>
       </c>
       <c r="D15">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E15">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="F15">
-        <v>26.03</v>
+        <v>31.73</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -916,13 +1155,13 @@
         <v>21</v>
       </c>
       <c r="D16">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E16">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="F16">
-        <v>45.83</v>
+        <v>43.99</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -936,13 +1175,13 @@
         <v>22</v>
       </c>
       <c r="D17">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E17">
-        <v>91</v>
+        <v>45</v>
       </c>
       <c r="F17">
-        <v>57.47</v>
+        <v>34.84</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -956,13 +1195,13 @@
         <v>23</v>
       </c>
       <c r="D18">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E18">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="F18">
-        <v>57.64</v>
+        <v>50.47</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -976,13 +1215,13 @@
         <v>24</v>
       </c>
       <c r="D19">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E19">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="F19">
-        <v>66.84</v>
+        <v>46.11</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -996,13 +1235,13 @@
         <v>25</v>
       </c>
       <c r="D20">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E20">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="F20">
-        <v>72.16</v>
+        <v>66.52</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1016,13 +1255,13 @@
         <v>26</v>
       </c>
       <c r="D21">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E21">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="F21">
-        <v>59.55</v>
+        <v>54.34</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1039,10 +1278,10 @@
         <v>5</v>
       </c>
       <c r="E22">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F22">
-        <v>45.59</v>
+        <v>33.73</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1056,13 +1295,13 @@
         <v>28</v>
       </c>
       <c r="D23">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E23">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="F23">
-        <v>26.9</v>
+        <v>41.71</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1076,13 +1315,13 @@
         <v>29</v>
       </c>
       <c r="D24">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E24">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F24">
-        <v>26.53</v>
+        <v>17.95</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1096,13 +1335,13 @@
         <v>30</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E25">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="F25">
-        <v>57.92</v>
+        <v>11.09</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1116,13 +1355,13 @@
         <v>31</v>
       </c>
       <c r="D26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E26">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="F26">
-        <v>41.34</v>
+        <v>36.19</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1136,13 +1375,13 @@
         <v>32</v>
       </c>
       <c r="D27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E27">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="F27">
-        <v>45.61</v>
+        <v>43.43</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1156,13 +1395,13 @@
         <v>33</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E28">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="F28">
-        <v>28.01</v>
+        <v>37.6</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1176,13 +1415,13 @@
         <v>34</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E29">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="F29">
-        <v>15.0</v>
+        <v>25.23</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1195,9 +1434,15 @@
       <c r="C30" t="s">
         <v>35</v>
       </c>
-      <c r="D30"/>
-      <c r="E30"/>
-      <c r="F30"/>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
@@ -1419,15 +1664,9 @@
       <c r="C46" t="s">
         <v>51</v>
       </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-      <c r="E46">
-        <v>7</v>
-      </c>
-      <c r="F46">
-        <v>4.17</v>
-      </c>
+      <c r="D46"/>
+      <c r="E46"/>
+      <c r="F46"/>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
@@ -1664,15 +1903,9 @@
       <c r="C7" t="s">
         <v>66</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>8</v>
-      </c>
-      <c r="F7">
-        <v>21.25</v>
-      </c>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
@@ -1685,13 +1918,13 @@
         <v>16</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="F8">
-        <v>28.65</v>
+        <v>3.13</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1705,13 +1938,13 @@
         <v>67</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="F9">
-        <v>29.77</v>
+        <v>22.43</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1725,13 +1958,13 @@
         <v>68</v>
       </c>
       <c r="D10">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="F10">
-        <v>51.41</v>
+        <v>29.37</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1745,13 +1978,13 @@
         <v>69</v>
       </c>
       <c r="D11">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E11">
-        <v>136</v>
+        <v>57</v>
       </c>
       <c r="F11">
-        <v>30.85</v>
+        <v>33.9</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1765,13 +1998,13 @@
         <v>70</v>
       </c>
       <c r="D12">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E12">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="F12">
-        <v>57.76</v>
+        <v>37.85</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1785,13 +2018,13 @@
         <v>71</v>
       </c>
       <c r="D13">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E13">
-        <v>125</v>
+        <v>62</v>
       </c>
       <c r="F13">
-        <v>52.65</v>
+        <v>46.62</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1805,13 +2038,13 @@
         <v>72</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E14">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="F14">
-        <v>75.17</v>
+        <v>55.17</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1825,13 +2058,13 @@
         <v>26</v>
       </c>
       <c r="D15">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E15">
-        <v>127</v>
+        <v>44</v>
       </c>
       <c r="F15">
-        <v>62.38</v>
+        <v>54.34</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1845,13 +2078,13 @@
         <v>73</v>
       </c>
       <c r="D16">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E16">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="F16">
-        <v>42.09</v>
+        <v>35.3</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1865,13 +2098,13 @@
         <v>74</v>
       </c>
       <c r="D17">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E17">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="F17">
-        <v>28.72</v>
+        <v>27.91</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1885,13 +2118,13 @@
         <v>75</v>
       </c>
       <c r="D18">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E18">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="F18">
-        <v>36.52</v>
+        <v>18.28</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1905,13 +2138,13 @@
         <v>76</v>
       </c>
       <c r="D19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E19">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="F19">
-        <v>56.5</v>
+        <v>44.83</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1925,13 +2158,13 @@
         <v>77</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E20">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="F20">
-        <v>30.64</v>
+        <v>33.27</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1945,13 +2178,13 @@
         <v>78</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="F21">
-        <v>15.0</v>
+        <v>19.92</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2118,15 +2351,9 @@
       <c r="C33" t="s">
         <v>88</v>
       </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33">
-        <v>7</v>
-      </c>
-      <c r="F33">
-        <v>4.17</v>
-      </c>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
@@ -2179,6 +2406,1550 @@
       </c>
       <c r="C37" t="s">
         <v>91</v>
+      </c>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:F53"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="true" style="0"/>
+    <col min="2" max="2" width="20" customWidth="true" style="0"/>
+    <col min="3" max="3" width="20" customWidth="true" style="0"/>
+    <col min="4" max="4" width="20" customWidth="true" style="0"/>
+    <col min="5" max="5" width="20" customWidth="true" style="0"/>
+    <col min="6" max="6" width="20" customWidth="true" style="0"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <v>15.83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>20</v>
+      </c>
+      <c r="F13">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>51</v>
+      </c>
+      <c r="F14">
+        <v>36.37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>44</v>
+      </c>
+      <c r="F15">
+        <v>44.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>41</v>
+      </c>
+      <c r="F16">
+        <v>13.46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>49</v>
+      </c>
+      <c r="F17">
+        <v>16.48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>40</v>
+      </c>
+      <c r="F18">
+        <v>28.05</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>58</v>
+      </c>
+      <c r="F19">
+        <v>49.19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>20</v>
+      </c>
+      <c r="F20">
+        <v>67.04</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>111</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <v>25</v>
+      </c>
+      <c r="F21">
+        <v>43.33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>49</v>
+      </c>
+      <c r="F22">
+        <v>61.17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+      <c r="E23">
+        <v>34</v>
+      </c>
+      <c r="F23">
+        <v>52.32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>29</v>
+      </c>
+      <c r="F24">
+        <v>46.81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <v>41</v>
+      </c>
+      <c r="F25">
+        <v>38.96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>116</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <v>29</v>
+      </c>
+      <c r="F26">
+        <v>32.56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>117</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>25</v>
+      </c>
+      <c r="F27">
+        <v>32.85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <v>23</v>
+      </c>
+      <c r="F28">
+        <v>59.07</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>119</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+      <c r="E29">
+        <v>30</v>
+      </c>
+      <c r="F29">
+        <v>31.41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>28</v>
+      </c>
+      <c r="F30">
+        <v>38.11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
+        <v>122</v>
+      </c>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33" t="s">
+        <v>123</v>
+      </c>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34" t="s">
+        <v>124</v>
+      </c>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35" t="s">
+        <v>125</v>
+      </c>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
+        <v>127</v>
+      </c>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38" t="s">
+        <v>128</v>
+      </c>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39" t="s">
+        <v>129</v>
+      </c>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40" t="s">
+        <v>130</v>
+      </c>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41" t="s">
+        <v>131</v>
+      </c>
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+      <c r="C42" t="s">
+        <v>132</v>
+      </c>
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+      <c r="C43" t="s">
+        <v>133</v>
+      </c>
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44">
+        <v>43</v>
+      </c>
+      <c r="C44" t="s">
+        <v>134</v>
+      </c>
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45">
+        <v>44</v>
+      </c>
+      <c r="C45" t="s">
+        <v>135</v>
+      </c>
+      <c r="D45"/>
+      <c r="E45"/>
+      <c r="F45"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
+      </c>
+      <c r="C46" t="s">
+        <v>136</v>
+      </c>
+      <c r="D46"/>
+      <c r="E46"/>
+      <c r="F46"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47">
+        <v>46</v>
+      </c>
+      <c r="C47" t="s">
+        <v>137</v>
+      </c>
+      <c r="D47"/>
+      <c r="E47"/>
+      <c r="F47"/>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48">
+        <v>47</v>
+      </c>
+      <c r="C48" t="s">
+        <v>138</v>
+      </c>
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48"/>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49">
+        <v>48</v>
+      </c>
+      <c r="C49" t="s">
+        <v>139</v>
+      </c>
+      <c r="D49"/>
+      <c r="E49"/>
+      <c r="F49"/>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50">
+        <v>49</v>
+      </c>
+      <c r="C50" t="s">
+        <v>140</v>
+      </c>
+      <c r="D50"/>
+      <c r="E50"/>
+      <c r="F50"/>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51">
+        <v>50</v>
+      </c>
+      <c r="C51" t="s">
+        <v>141</v>
+      </c>
+      <c r="D51"/>
+      <c r="E51"/>
+      <c r="F51"/>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52">
+        <v>51</v>
+      </c>
+      <c r="C52" t="s">
+        <v>142</v>
+      </c>
+      <c r="D52"/>
+      <c r="E52"/>
+      <c r="F52"/>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53">
+        <v>52</v>
+      </c>
+      <c r="C53" t="s">
+        <v>143</v>
+      </c>
+      <c r="D53"/>
+      <c r="E53"/>
+      <c r="F53"/>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:F37"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="true" style="0"/>
+    <col min="2" max="2" width="20" customWidth="true" style="0"/>
+    <col min="3" max="3" width="20" customWidth="true" style="0"/>
+    <col min="4" max="4" width="20" customWidth="true" style="0"/>
+    <col min="5" max="5" width="20" customWidth="true" style="0"/>
+    <col min="6" max="6" width="20" customWidth="true" style="0"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <v>15.83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>71</v>
+      </c>
+      <c r="F10">
+        <v>31.65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>152</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>53</v>
+      </c>
+      <c r="F11">
+        <v>35.96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>46</v>
+      </c>
+      <c r="F12">
+        <v>19.13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>154</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>75</v>
+      </c>
+      <c r="F13">
+        <v>21.97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>155</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>78</v>
+      </c>
+      <c r="F14">
+        <v>56.33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>25</v>
+      </c>
+      <c r="F15">
+        <v>43.33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>49</v>
+      </c>
+      <c r="F16">
+        <v>61.17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>49</v>
+      </c>
+      <c r="F17">
+        <v>46.68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>158</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>70</v>
+      </c>
+      <c r="F18">
+        <v>42.08</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>159</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>22</v>
+      </c>
+      <c r="F19">
+        <v>29.06</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>160</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <v>51</v>
+      </c>
+      <c r="F20">
+        <v>51.01</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>161</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <v>30</v>
+      </c>
+      <c r="F21">
+        <v>27.99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>17</v>
+      </c>
+      <c r="F22">
+        <v>49.79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>163</v>
+      </c>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>164</v>
+      </c>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>165</v>
+      </c>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>166</v>
+      </c>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>167</v>
+      </c>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>131</v>
+      </c>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>168</v>
+      </c>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>169</v>
+      </c>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
+        <v>170</v>
+      </c>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33" t="s">
+        <v>171</v>
+      </c>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34" t="s">
+        <v>172</v>
+      </c>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35" t="s">
+        <v>173</v>
+      </c>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>141</v>
+      </c>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
+        <v>174</v>
       </c>
       <c r="D37"/>
       <c r="E37"/>

</xml_diff>

<commit_message>
Modification et validation de la fonction trouverMesuresParcelles
</commit_message>
<xml_diff>
--- a/fichierInter.xlsx
+++ b/fichierInter.xlsx
@@ -38,7 +38,7 @@
     <t>Date début semaine</t>
   </si>
   <si>
-    <t>Adice</t>
+    <t>Montagne</t>
   </si>
   <si>
     <t>07/01/2020</t>
@@ -1054,15 +1054,9 @@
       <c r="C11" t="s">
         <v>16</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>18</v>
-      </c>
-      <c r="F11">
-        <v>3.13</v>
-      </c>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
@@ -1075,13 +1069,13 @@
         <v>17</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="F12">
-        <v>17.68</v>
+        <v>5.95</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1098,10 +1092,10 @@
         <v>2</v>
       </c>
       <c r="E13">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F13">
-        <v>25.98</v>
+        <v>19.83</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1115,13 +1109,13 @@
         <v>19</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="F14">
-        <v>28.51</v>
+        <v>21.89</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1138,10 +1132,10 @@
         <v>3</v>
       </c>
       <c r="E15">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F15">
-        <v>31.73</v>
+        <v>22.54</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1158,10 +1152,10 @@
         <v>4</v>
       </c>
       <c r="E16">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F16">
-        <v>43.99</v>
+        <v>36.49</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1178,10 +1172,10 @@
         <v>4</v>
       </c>
       <c r="E17">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F17">
-        <v>34.84</v>
+        <v>31.13</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1195,13 +1189,13 @@
         <v>23</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E18">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F18">
-        <v>50.47</v>
+        <v>76.97</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1218,10 +1212,10 @@
         <v>5</v>
       </c>
       <c r="E19">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="F19">
-        <v>46.11</v>
+        <v>55.58</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1238,10 +1232,10 @@
         <v>4</v>
       </c>
       <c r="E20">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="F20">
-        <v>66.52</v>
+        <v>76.89</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1255,13 +1249,13 @@
         <v>26</v>
       </c>
       <c r="D21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E21">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="F21">
-        <v>54.34</v>
+        <v>63.2</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1278,10 +1272,10 @@
         <v>5</v>
       </c>
       <c r="E22">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="F22">
-        <v>33.73</v>
+        <v>43.22</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1298,10 +1292,10 @@
         <v>5</v>
       </c>
       <c r="E23">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="F23">
-        <v>41.71</v>
+        <v>31.95</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1321,7 +1315,7 @@
         <v>28</v>
       </c>
       <c r="F24">
-        <v>17.95</v>
+        <v>20.52</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1335,13 +1329,13 @@
         <v>30</v>
       </c>
       <c r="D25">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E25">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="F25">
-        <v>11.09</v>
+        <v>13.18</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1355,13 +1349,13 @@
         <v>31</v>
       </c>
       <c r="D26">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E26">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="F26">
-        <v>36.19</v>
+        <v>32.02</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1375,13 +1369,13 @@
         <v>32</v>
       </c>
       <c r="D27">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E27">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F27">
-        <v>43.43</v>
+        <v>33.3</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1395,13 +1389,13 @@
         <v>33</v>
       </c>
       <c r="D28">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E28">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="F28">
-        <v>37.6</v>
+        <v>26.48</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1415,13 +1409,13 @@
         <v>34</v>
       </c>
       <c r="D29">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E29">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="F29">
-        <v>25.23</v>
+        <v>39.36</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1438,10 +1432,10 @@
         <v>1</v>
       </c>
       <c r="E30">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F30">
-        <v>0.0</v>
+        <v>27.04</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1454,9 +1448,15 @@
       <c r="C31" t="s">
         <v>36</v>
       </c>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>6</v>
+      </c>
+      <c r="F31">
+        <v>27.61</v>
+      </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
@@ -1917,15 +1917,9 @@
       <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>18</v>
-      </c>
-      <c r="F8">
-        <v>3.13</v>
-      </c>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
@@ -1938,13 +1932,13 @@
         <v>67</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="F9">
-        <v>22.43</v>
+        <v>6.42</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1961,10 +1955,10 @@
         <v>2</v>
       </c>
       <c r="E10">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F10">
-        <v>29.37</v>
+        <v>26.31</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1981,10 +1975,10 @@
         <v>3</v>
       </c>
       <c r="E11">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F11">
-        <v>33.9</v>
+        <v>22.37</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2001,10 +1995,10 @@
         <v>4</v>
       </c>
       <c r="E12">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F12">
-        <v>37.85</v>
+        <v>35.52</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2021,10 +2015,10 @@
         <v>4</v>
       </c>
       <c r="E13">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="F13">
-        <v>46.62</v>
+        <v>60.61</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2041,10 +2035,10 @@
         <v>5</v>
       </c>
       <c r="E14">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="F14">
-        <v>55.17</v>
+        <v>65.55</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2061,10 +2055,10 @@
         <v>5</v>
       </c>
       <c r="E15">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="F15">
-        <v>54.34</v>
+        <v>68.3</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2081,10 +2075,10 @@
         <v>5</v>
       </c>
       <c r="E16">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F16">
-        <v>35.3</v>
+        <v>41.17</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2101,10 +2095,10 @@
         <v>5</v>
       </c>
       <c r="E17">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F17">
-        <v>27.91</v>
+        <v>23.16</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2118,13 +2112,13 @@
         <v>75</v>
       </c>
       <c r="D18">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E18">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="F18">
-        <v>18.28</v>
+        <v>17.99</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2138,13 +2132,13 @@
         <v>76</v>
       </c>
       <c r="D19">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E19">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F19">
-        <v>44.83</v>
+        <v>39.01</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2158,13 +2152,13 @@
         <v>77</v>
       </c>
       <c r="D20">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E20">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="F20">
-        <v>33.27</v>
+        <v>26.48</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2181,10 +2175,10 @@
         <v>2</v>
       </c>
       <c r="E21">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F21">
-        <v>19.92</v>
+        <v>35.25</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2197,9 +2191,15 @@
       <c r="C22" t="s">
         <v>36</v>
       </c>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>6</v>
+      </c>
+      <c r="F22">
+        <v>27.61</v>
+      </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
@@ -2618,15 +2618,9 @@
       <c r="C12" t="s">
         <v>102</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>15</v>
-      </c>
-      <c r="F12">
-        <v>15.83</v>
-      </c>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
@@ -2639,13 +2633,13 @@
         <v>103</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F13">
-        <v>17.5</v>
+        <v>19.46</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2662,10 +2656,10 @@
         <v>4</v>
       </c>
       <c r="E14">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F14">
-        <v>36.37</v>
+        <v>19.69</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2679,13 +2673,13 @@
         <v>105</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E15">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="F15">
-        <v>44.7</v>
+        <v>43.18</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2702,10 +2696,10 @@
         <v>3</v>
       </c>
       <c r="E16">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="F16">
-        <v>13.46</v>
+        <v>13.32</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2719,13 +2713,13 @@
         <v>107</v>
       </c>
       <c r="D17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E17">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="F17">
-        <v>16.48</v>
+        <v>17.53</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2745,7 +2739,7 @@
         <v>40</v>
       </c>
       <c r="F18">
-        <v>28.05</v>
+        <v>38.53</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2759,13 +2753,13 @@
         <v>109</v>
       </c>
       <c r="D19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E19">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="F19">
-        <v>49.19</v>
+        <v>38.34</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2779,13 +2773,13 @@
         <v>110</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F20">
-        <v>67.04</v>
+        <v>59.55</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2802,10 +2796,10 @@
         <v>4</v>
       </c>
       <c r="E21">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F21">
-        <v>43.33</v>
+        <v>63.1</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2819,13 +2813,13 @@
         <v>112</v>
       </c>
       <c r="D22">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E22">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="F22">
-        <v>61.17</v>
+        <v>50.18</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2842,10 +2836,10 @@
         <v>5</v>
       </c>
       <c r="E23">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="F23">
-        <v>52.32</v>
+        <v>40.66</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2859,13 +2853,13 @@
         <v>114</v>
       </c>
       <c r="D24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E24">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F24">
-        <v>46.81</v>
+        <v>59.96</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2879,13 +2873,13 @@
         <v>115</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E25">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F25">
-        <v>38.96</v>
+        <v>42.37</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2902,10 +2896,10 @@
         <v>4</v>
       </c>
       <c r="E26">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F26">
-        <v>32.56</v>
+        <v>39.55</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2919,13 +2913,13 @@
         <v>117</v>
       </c>
       <c r="D27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E27">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="F27">
-        <v>32.85</v>
+        <v>32.31</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2939,13 +2933,13 @@
         <v>118</v>
       </c>
       <c r="D28">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E28">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="F28">
-        <v>59.07</v>
+        <v>34.52</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2959,13 +2953,13 @@
         <v>119</v>
       </c>
       <c r="D29">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E29">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="F29">
-        <v>31.41</v>
+        <v>28.85</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2978,15 +2972,9 @@
       <c r="C30" t="s">
         <v>120</v>
       </c>
-      <c r="D30">
-        <v>2</v>
-      </c>
-      <c r="E30">
-        <v>28</v>
-      </c>
-      <c r="F30">
-        <v>38.11</v>
-      </c>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
@@ -3068,9 +3056,15 @@
       <c r="C36" t="s">
         <v>126</v>
       </c>
-      <c r="D36"/>
-      <c r="E36"/>
-      <c r="F36"/>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>6</v>
+      </c>
+      <c r="F36">
+        <v>12.5</v>
+      </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
@@ -3082,9 +3076,15 @@
       <c r="C37" t="s">
         <v>127</v>
       </c>
-      <c r="D37"/>
-      <c r="E37"/>
-      <c r="F37"/>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>4</v>
+      </c>
+      <c r="F37">
+        <v>32.14</v>
+      </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
@@ -3096,9 +3096,15 @@
       <c r="C38" t="s">
         <v>128</v>
       </c>
-      <c r="D38"/>
-      <c r="E38"/>
-      <c r="F38"/>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>21.43</v>
+      </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
@@ -3110,9 +3116,15 @@
       <c r="C39" t="s">
         <v>129</v>
       </c>
-      <c r="D39"/>
-      <c r="E39"/>
-      <c r="F39"/>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>3</v>
+      </c>
+      <c r="F39">
+        <v>20.24</v>
+      </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
@@ -3124,9 +3136,15 @@
       <c r="C40" t="s">
         <v>130</v>
       </c>
-      <c r="D40"/>
-      <c r="E40"/>
-      <c r="F40"/>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>4</v>
+      </c>
+      <c r="F40">
+        <v>17.86</v>
+      </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
@@ -3152,9 +3170,15 @@
       <c r="C42" t="s">
         <v>132</v>
       </c>
-      <c r="D42"/>
-      <c r="E42"/>
-      <c r="F42"/>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>4</v>
+      </c>
+      <c r="F42">
+        <v>15.18</v>
+      </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
@@ -3479,10 +3503,10 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>15.83</v>
+        <v>19.46</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3499,10 +3523,10 @@
         <v>4</v>
       </c>
       <c r="E10">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="F10">
-        <v>31.65</v>
+        <v>19.69</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -3519,10 +3543,10 @@
         <v>4</v>
       </c>
       <c r="E11">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F11">
-        <v>35.96</v>
+        <v>37.12</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -3539,10 +3563,10 @@
         <v>4</v>
       </c>
       <c r="E12">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="F12">
-        <v>19.13</v>
+        <v>15.83</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3559,10 +3583,10 @@
         <v>5</v>
       </c>
       <c r="E13">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="F13">
-        <v>21.97</v>
+        <v>30.07</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -3576,13 +3600,13 @@
         <v>155</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E14">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="F14">
-        <v>56.33</v>
+        <v>54.09</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -3599,10 +3623,10 @@
         <v>4</v>
       </c>
       <c r="E15">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F15">
-        <v>43.33</v>
+        <v>61.17</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -3616,13 +3640,13 @@
         <v>156</v>
       </c>
       <c r="D16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E16">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F16">
-        <v>61.17</v>
+        <v>52.33</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -3639,10 +3663,10 @@
         <v>5</v>
       </c>
       <c r="E17">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F17">
-        <v>46.68</v>
+        <v>41.86</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -3656,13 +3680,13 @@
         <v>158</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E18">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F18">
-        <v>42.08</v>
+        <v>44.79</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -3676,13 +3700,13 @@
         <v>159</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E19">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="F19">
-        <v>29.06</v>
+        <v>34.95</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -3696,13 +3720,13 @@
         <v>160</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E20">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F20">
-        <v>51.01</v>
+        <v>27.82</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -3716,13 +3740,13 @@
         <v>161</v>
       </c>
       <c r="D21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="F21">
-        <v>27.99</v>
+        <v>43.75</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -3735,15 +3759,9 @@
       <c r="C22" t="s">
         <v>121</v>
       </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>17</v>
-      </c>
-      <c r="F22">
-        <v>49.79</v>
-      </c>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
@@ -3783,9 +3801,15 @@
       <c r="C25" t="s">
         <v>164</v>
       </c>
-      <c r="D25"/>
-      <c r="E25"/>
-      <c r="F25"/>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>6</v>
+      </c>
+      <c r="F25">
+        <v>12.5</v>
+      </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
@@ -3797,9 +3821,15 @@
       <c r="C26" t="s">
         <v>165</v>
       </c>
-      <c r="D26"/>
-      <c r="E26"/>
-      <c r="F26"/>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <v>32.14</v>
+      </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
@@ -3811,9 +3841,15 @@
       <c r="C27" t="s">
         <v>166</v>
       </c>
-      <c r="D27"/>
-      <c r="E27"/>
-      <c r="F27"/>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <v>20.84</v>
+      </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
@@ -3825,9 +3861,15 @@
       <c r="C28" t="s">
         <v>167</v>
       </c>
-      <c r="D28"/>
-      <c r="E28"/>
-      <c r="F28"/>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <v>17.86</v>
+      </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
@@ -3853,9 +3895,15 @@
       <c r="C30" t="s">
         <v>168</v>
       </c>
-      <c r="D30"/>
-      <c r="E30"/>
-      <c r="F30"/>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+      <c r="F30">
+        <v>15.18</v>
+      </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">

</xml_diff>

<commit_message>
Factorisation de la fonction calculMoyenne et creation de la fonction de factorisation creationSheetRes pour choix exploitations
</commit_message>
<xml_diff>
--- a/fichierInter.xlsx
+++ b/fichierInter.xlsx
@@ -38,7 +38,7 @@
     <t>Date début semaine</t>
   </si>
   <si>
-    <t>Montagne</t>
+    <t>Plaine</t>
   </si>
   <si>
     <t>07/01/2020</t>
@@ -1026,9 +1026,15 @@
       <c r="C9" t="s">
         <v>14</v>
       </c>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>21.25</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
@@ -1040,9 +1046,15 @@
       <c r="C10" t="s">
         <v>15</v>
       </c>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>17</v>
+      </c>
+      <c r="F10">
+        <v>15.13</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
@@ -1054,9 +1066,15 @@
       <c r="C11" t="s">
         <v>16</v>
       </c>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>24</v>
+      </c>
+      <c r="F11">
+        <v>35.42</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
@@ -1069,13 +1087,13 @@
         <v>17</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F12">
-        <v>5.95</v>
+        <v>25.89</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1089,13 +1107,13 @@
         <v>18</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E13">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="F13">
-        <v>19.83</v>
+        <v>51.02</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1109,13 +1127,13 @@
         <v>19</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E14">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="F14">
-        <v>21.89</v>
+        <v>38.4</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1129,13 +1147,13 @@
         <v>20</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E15">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="F15">
-        <v>22.54</v>
+        <v>26.03</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1149,13 +1167,13 @@
         <v>21</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E16">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="F16">
-        <v>36.49</v>
+        <v>45.83</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1169,13 +1187,13 @@
         <v>22</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E17">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="F17">
-        <v>31.13</v>
+        <v>57.47</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1189,13 +1207,13 @@
         <v>23</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E18">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="F18">
-        <v>76.97</v>
+        <v>57.64</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1209,13 +1227,13 @@
         <v>24</v>
       </c>
       <c r="D19">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E19">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="F19">
-        <v>55.58</v>
+        <v>66.84</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1229,13 +1247,13 @@
         <v>25</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E20">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="F20">
-        <v>76.89</v>
+        <v>72.16</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1249,13 +1267,13 @@
         <v>26</v>
       </c>
       <c r="D21">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E21">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="F21">
-        <v>63.2</v>
+        <v>59.55</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1272,10 +1290,10 @@
         <v>5</v>
       </c>
       <c r="E22">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="F22">
-        <v>43.22</v>
+        <v>45.59</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1289,13 +1307,13 @@
         <v>28</v>
       </c>
       <c r="D23">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E23">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F23">
-        <v>31.95</v>
+        <v>26.9</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1309,13 +1327,13 @@
         <v>29</v>
       </c>
       <c r="D24">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E24">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F24">
-        <v>20.52</v>
+        <v>26.53</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1329,13 +1347,13 @@
         <v>30</v>
       </c>
       <c r="D25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E25">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F25">
-        <v>13.18</v>
+        <v>57.92</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1349,13 +1367,13 @@
         <v>31</v>
       </c>
       <c r="D26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E26">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F26">
-        <v>32.02</v>
+        <v>41.34</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1369,13 +1387,13 @@
         <v>32</v>
       </c>
       <c r="D27">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E27">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F27">
-        <v>33.3</v>
+        <v>45.61</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1389,13 +1407,13 @@
         <v>33</v>
       </c>
       <c r="D28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E28">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="F28">
-        <v>26.48</v>
+        <v>28.01</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1409,13 +1427,13 @@
         <v>34</v>
       </c>
       <c r="D29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F29">
-        <v>39.36</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1428,15 +1446,9 @@
       <c r="C30" t="s">
         <v>35</v>
       </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30">
-        <v>7</v>
-      </c>
-      <c r="F30">
-        <v>27.04</v>
-      </c>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
@@ -1448,15 +1460,9 @@
       <c r="C31" t="s">
         <v>36</v>
       </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <v>6</v>
-      </c>
-      <c r="F31">
-        <v>27.61</v>
-      </c>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
@@ -1664,9 +1670,15 @@
       <c r="C46" t="s">
         <v>51</v>
       </c>
-      <c r="D46"/>
-      <c r="E46"/>
-      <c r="F46"/>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>7</v>
+      </c>
+      <c r="F46">
+        <v>4.17</v>
+      </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
@@ -1903,9 +1915,15 @@
       <c r="C7" t="s">
         <v>66</v>
       </c>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>21.25</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
@@ -1917,9 +1935,15 @@
       <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>41</v>
+      </c>
+      <c r="F8">
+        <v>28.65</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
@@ -1932,13 +1956,13 @@
         <v>67</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E9">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F9">
-        <v>6.42</v>
+        <v>29.77</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1952,13 +1976,13 @@
         <v>68</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E10">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="F10">
-        <v>26.31</v>
+        <v>51.41</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1972,13 +1996,13 @@
         <v>69</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E11">
-        <v>50</v>
+        <v>136</v>
       </c>
       <c r="F11">
-        <v>22.37</v>
+        <v>30.85</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1992,13 +2016,13 @@
         <v>70</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E12">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="F12">
-        <v>35.52</v>
+        <v>57.76</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2012,13 +2036,13 @@
         <v>71</v>
       </c>
       <c r="D13">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E13">
-        <v>77</v>
+        <v>125</v>
       </c>
       <c r="F13">
-        <v>60.61</v>
+        <v>52.65</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2032,13 +2056,13 @@
         <v>72</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E14">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="F14">
-        <v>65.55</v>
+        <v>75.17</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2052,13 +2076,13 @@
         <v>26</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E15">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="F15">
-        <v>68.3</v>
+        <v>62.38</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2072,13 +2096,13 @@
         <v>73</v>
       </c>
       <c r="D16">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E16">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="F16">
-        <v>41.17</v>
+        <v>42.09</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2092,13 +2116,13 @@
         <v>74</v>
       </c>
       <c r="D17">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E17">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="F17">
-        <v>23.16</v>
+        <v>28.72</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2112,13 +2136,13 @@
         <v>75</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E18">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="F18">
-        <v>17.99</v>
+        <v>36.52</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2132,13 +2156,13 @@
         <v>76</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E19">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F19">
-        <v>39.01</v>
+        <v>56.5</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2152,13 +2176,13 @@
         <v>77</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E20">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="F20">
-        <v>26.48</v>
+        <v>30.64</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2172,13 +2196,13 @@
         <v>78</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="F21">
-        <v>35.25</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2191,15 +2215,9 @@
       <c r="C22" t="s">
         <v>36</v>
       </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>6</v>
-      </c>
-      <c r="F22">
-        <v>27.61</v>
-      </c>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
@@ -2351,9 +2369,15 @@
       <c r="C33" t="s">
         <v>88</v>
       </c>
-      <c r="D33"/>
-      <c r="E33"/>
-      <c r="F33"/>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>7</v>
+      </c>
+      <c r="F33">
+        <v>4.17</v>
+      </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
@@ -2604,9 +2628,15 @@
       <c r="C11" t="s">
         <v>101</v>
       </c>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>21</v>
+      </c>
+      <c r="F11">
+        <v>14.15</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
@@ -2618,9 +2648,15 @@
       <c r="C12" t="s">
         <v>102</v>
       </c>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>55</v>
+      </c>
+      <c r="F12">
+        <v>20.18</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
@@ -2633,13 +2669,13 @@
         <v>103</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E13">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="F13">
-        <v>19.46</v>
+        <v>24.31</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2653,13 +2689,13 @@
         <v>104</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E14">
-        <v>45</v>
+        <v>166</v>
       </c>
       <c r="F14">
-        <v>19.69</v>
+        <v>32.94</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2673,13 +2709,13 @@
         <v>105</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E15">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="F15">
-        <v>43.18</v>
+        <v>44.95</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2693,13 +2729,13 @@
         <v>106</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E16">
-        <v>28</v>
+        <v>112</v>
       </c>
       <c r="F16">
-        <v>13.32</v>
+        <v>42.3</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2713,13 +2749,13 @@
         <v>107</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E17">
-        <v>29</v>
+        <v>127</v>
       </c>
       <c r="F17">
-        <v>17.53</v>
+        <v>34.39</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2733,13 +2769,13 @@
         <v>108</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E18">
-        <v>40</v>
+        <v>108</v>
       </c>
       <c r="F18">
-        <v>38.53</v>
+        <v>49.96</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2753,13 +2789,13 @@
         <v>109</v>
       </c>
       <c r="D19">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E19">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="F19">
-        <v>38.34</v>
+        <v>69.17</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2773,13 +2809,13 @@
         <v>110</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E20">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="F20">
-        <v>59.55</v>
+        <v>70.15</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2793,13 +2829,13 @@
         <v>111</v>
       </c>
       <c r="D21">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E21">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="F21">
-        <v>63.1</v>
+        <v>81.56</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2813,13 +2849,13 @@
         <v>112</v>
       </c>
       <c r="D22">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E22">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="F22">
-        <v>50.18</v>
+        <v>51.85</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2833,13 +2869,13 @@
         <v>113</v>
       </c>
       <c r="D23">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E23">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="F23">
-        <v>40.66</v>
+        <v>53.65</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2853,13 +2889,13 @@
         <v>114</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E24">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F24">
-        <v>59.96</v>
+        <v>49.95</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2873,13 +2909,13 @@
         <v>115</v>
       </c>
       <c r="D25">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E25">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F25">
-        <v>42.37</v>
+        <v>89.1</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2893,13 +2929,13 @@
         <v>116</v>
       </c>
       <c r="D26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E26">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="F26">
-        <v>39.55</v>
+        <v>40.42</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2913,13 +2949,13 @@
         <v>117</v>
       </c>
       <c r="D27">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E27">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F27">
-        <v>32.31</v>
+        <v>51.68</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2933,13 +2969,13 @@
         <v>118</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E28">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="F28">
-        <v>34.52</v>
+        <v>48.14</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2953,13 +2989,13 @@
         <v>119</v>
       </c>
       <c r="D29">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E29">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="F29">
-        <v>28.85</v>
+        <v>71.43</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2972,9 +3008,15 @@
       <c r="C30" t="s">
         <v>120</v>
       </c>
-      <c r="D30"/>
-      <c r="E30"/>
-      <c r="F30"/>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>10</v>
+      </c>
+      <c r="F30">
+        <v>46.87</v>
+      </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
@@ -2986,9 +3028,15 @@
       <c r="C31" t="s">
         <v>121</v>
       </c>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>5</v>
+      </c>
+      <c r="F31">
+        <v>21.43</v>
+      </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
@@ -3014,9 +3062,15 @@
       <c r="C33" t="s">
         <v>123</v>
       </c>
-      <c r="D33"/>
-      <c r="E33"/>
-      <c r="F33"/>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+      <c r="F33">
+        <v>44.05</v>
+      </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
@@ -3028,9 +3082,15 @@
       <c r="C34" t="s">
         <v>124</v>
       </c>
-      <c r="D34"/>
-      <c r="E34"/>
-      <c r="F34"/>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>6</v>
+      </c>
+      <c r="F34">
+        <v>54.63</v>
+      </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
@@ -3042,9 +3102,15 @@
       <c r="C35" t="s">
         <v>125</v>
       </c>
-      <c r="D35"/>
-      <c r="E35"/>
-      <c r="F35"/>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>7</v>
+      </c>
+      <c r="F35">
+        <v>33.48</v>
+      </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
@@ -3057,13 +3123,13 @@
         <v>126</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E36">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F36">
-        <v>12.5</v>
+        <v>15.14</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -3080,10 +3146,10 @@
         <v>1</v>
       </c>
       <c r="E37">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37">
-        <v>32.14</v>
+        <v>73.61</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -3096,15 +3162,9 @@
       <c r="C38" t="s">
         <v>128</v>
       </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="F38">
-        <v>21.43</v>
-      </c>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
@@ -3120,10 +3180,10 @@
         <v>1</v>
       </c>
       <c r="E39">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F39">
-        <v>20.24</v>
+        <v>30.59</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -3136,15 +3196,9 @@
       <c r="C40" t="s">
         <v>130</v>
       </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="E40">
-        <v>4</v>
-      </c>
-      <c r="F40">
-        <v>17.86</v>
-      </c>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
@@ -3156,9 +3210,15 @@
       <c r="C41" t="s">
         <v>131</v>
       </c>
-      <c r="D41"/>
-      <c r="E41"/>
-      <c r="F41"/>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>6</v>
+      </c>
+      <c r="F41">
+        <v>22.92</v>
+      </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
@@ -3174,10 +3234,10 @@
         <v>1</v>
       </c>
       <c r="E42">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F42">
-        <v>15.18</v>
+        <v>23.47</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -3190,9 +3250,15 @@
       <c r="C43" t="s">
         <v>133</v>
       </c>
-      <c r="D43"/>
-      <c r="E43"/>
-      <c r="F43"/>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>6</v>
+      </c>
+      <c r="F43">
+        <v>12.12</v>
+      </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
@@ -3485,9 +3551,15 @@
       <c r="C8" t="s">
         <v>101</v>
       </c>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>21</v>
+      </c>
+      <c r="F8">
+        <v>14.15</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
@@ -3500,13 +3572,13 @@
         <v>150</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E9">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="F9">
-        <v>19.46</v>
+        <v>18.53</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3520,13 +3592,13 @@
         <v>151</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E10">
-        <v>45</v>
+        <v>169</v>
       </c>
       <c r="F10">
-        <v>19.69</v>
+        <v>33.02</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -3540,13 +3612,13 @@
         <v>152</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E11">
-        <v>47</v>
+        <v>146</v>
       </c>
       <c r="F11">
-        <v>37.12</v>
+        <v>40.35</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -3560,13 +3632,13 @@
         <v>153</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E12">
-        <v>29</v>
+        <v>145</v>
       </c>
       <c r="F12">
-        <v>15.83</v>
+        <v>38.55</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3580,13 +3652,13 @@
         <v>154</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E13">
-        <v>56</v>
+        <v>179</v>
       </c>
       <c r="F13">
-        <v>30.07</v>
+        <v>50.58</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -3600,13 +3672,13 @@
         <v>155</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E14">
-        <v>49</v>
+        <v>130</v>
       </c>
       <c r="F14">
-        <v>54.09</v>
+        <v>69.06</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -3620,13 +3692,13 @@
         <v>111</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E15">
-        <v>35</v>
+        <v>123</v>
       </c>
       <c r="F15">
-        <v>61.17</v>
+        <v>78.95</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -3640,13 +3712,13 @@
         <v>156</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E16">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="F16">
-        <v>52.33</v>
+        <v>53.03</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -3660,13 +3732,13 @@
         <v>157</v>
       </c>
       <c r="D17">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E17">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="F17">
-        <v>41.86</v>
+        <v>55.49</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -3680,13 +3752,13 @@
         <v>158</v>
       </c>
       <c r="D18">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E18">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F18">
-        <v>44.79</v>
+        <v>76.41</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -3700,13 +3772,13 @@
         <v>159</v>
       </c>
       <c r="D19">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E19">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="F19">
-        <v>34.95</v>
+        <v>43.41</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -3720,13 +3792,13 @@
         <v>160</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E20">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="F20">
-        <v>27.82</v>
+        <v>50.59</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -3746,7 +3818,7 @@
         <v>7</v>
       </c>
       <c r="F21">
-        <v>43.75</v>
+        <v>64.58</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -3759,9 +3831,15 @@
       <c r="C22" t="s">
         <v>121</v>
       </c>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>8</v>
+      </c>
+      <c r="F22">
+        <v>25.3</v>
+      </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
@@ -3787,9 +3865,15 @@
       <c r="C24" t="s">
         <v>163</v>
       </c>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24"/>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>9</v>
+      </c>
+      <c r="F24">
+        <v>49.34</v>
+      </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
@@ -3805,10 +3889,10 @@
         <v>1</v>
       </c>
       <c r="E25">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F25">
-        <v>12.5</v>
+        <v>33.48</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -3822,13 +3906,13 @@
         <v>165</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E26">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="F26">
-        <v>32.14</v>
+        <v>44.38</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -3845,10 +3929,10 @@
         <v>1</v>
       </c>
       <c r="E27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F27">
-        <v>20.84</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -3865,10 +3949,10 @@
         <v>1</v>
       </c>
       <c r="E28">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F28">
-        <v>17.86</v>
+        <v>41.67</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -3881,9 +3965,15 @@
       <c r="C29" t="s">
         <v>131</v>
       </c>
-      <c r="D29"/>
-      <c r="E29"/>
-      <c r="F29"/>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>6</v>
+      </c>
+      <c r="F29">
+        <v>22.92</v>
+      </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
@@ -3899,10 +3989,10 @@
         <v>1</v>
       </c>
       <c r="E30">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F30">
-        <v>15.18</v>
+        <v>23.47</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -3915,9 +4005,15 @@
       <c r="C31" t="s">
         <v>169</v>
       </c>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>6</v>
+      </c>
+      <c r="F31">
+        <v>12.12</v>
+      </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">

</xml_diff>